<commit_message>
Update excel workbook graphs (used in report)
</commit_message>
<xml_diff>
--- a/results/ugrad-009-01/ugrad-009-01-stats-identi-20.xlsx
+++ b/results/ugrad-009-01/ugrad-009-01-stats-identi-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desti\Documents\GitHub\P4P\results\ugrad-009-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2D74F8-9A64-41D2-870A-852F6931FEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF1BFCA-4019-473A-B9C1-566F5EE95320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,12 +709,81 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'ugrad-009-01-stats-20'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ugrad-009-01-stats-20'!$G$2:$G$22</c:f>
+              <c:f>'ugrad-009-01-stats-20'!$G$2:$G$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.44444444444444442</c:v>
                 </c:pt>
@@ -774,9 +843,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.41911764705882354</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.42570070124167297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,12 +877,81 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'ugrad-009-01-stats-20'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ugrad-009-01-stats-20'!$H$2:$H$22</c:f>
+              <c:f>'ugrad-009-01-stats-20'!$H$2:$H$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.51515151515151514</c:v>
                 </c:pt>
@@ -876,9 +1011,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.48529411764705882</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.50933879745217214</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,12 +1045,81 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'ugrad-009-01-stats-20'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1019</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ugrad-009-01-stats-20'!$I$2:$I$22</c:f>
+              <c:f>'ugrad-009-01-stats-20'!$I$2:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>4.0404040404040407E-2</c:v>
                 </c:pt>
@@ -978,9 +1179,6 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>9.5588235294117641E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.4960501306154855E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1011,6 +1209,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2076,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2F3F05-6040-485E-941D-4098ABFA4C94}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C21"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>